<commit_message>
atualiza script do grid
</commit_message>
<xml_diff>
--- a/grid_letras.xlsx
+++ b/grid_letras.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.pereira\Documents\GitHub\garantias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC12EE90-8313-436B-AF1E-53F3B9CA0103}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6475E4DB-F14D-4873-9BF0-FC86A28C8744}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{A7340747-A47E-4DC9-B3EB-D99C483E4830}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{A7340747-A47E-4DC9-B3EB-D99C483E4830}"/>
   </bookViews>
   <sheets>
     <sheet name="grid_teste" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="9" r:id="rId2"/>
+    <sheet name="tesouro" sheetId="9" r:id="rId2"/>
     <sheet name="grid_export" sheetId="2" r:id="rId3"/>
     <sheet name="export_2" sheetId="3" r:id="rId4"/>
     <sheet name="export_3" sheetId="4" r:id="rId5"/>
@@ -11055,8 +11055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DBD622-D758-4625-8498-E5473EF9EDAA}">
   <dimension ref="A1:BB134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:BA42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -16478,7 +16478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120E8356-7322-4EE4-892F-5BF5F2F2C56E}">
   <dimension ref="A1:BC46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>